<commit_message>
[update] format summonses header
</commit_message>
<xml_diff>
--- a/data/fare-evasions-summonses-2018-2023.xlsx
+++ b/data/fare-evasions-summonses-2018-2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D-Drive Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\mta-crime\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CEA1D3-A9C4-4C58-88D6-1C4C4570131E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFEF0CA-B8EC-4D4E-981B-9F30D809B50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="975" windowWidth="22635" windowHeight="14070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,12 +45,6 @@
   </si>
   <si>
     <t>Quarter End Date</t>
-  </si>
-  <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
-    <t>MALE</t>
   </si>
   <si>
     <t>American Indian</t>
@@ -96,6 +90,12 @@
   </si>
   <si>
     <t>Unknown-Gender</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -159,15 +159,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,64 +463,64 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" t="s">
         <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>